<commit_message>
Change Duration of Wait Time In Excel Config
</commit_message>
<xml_diff>
--- a/Data/config.xlsx
+++ b/Data/config.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24201"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DFE5238-9386-4A47-9E5C-AC4FB5204ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{880F78DE-CB5C-425D-BD0D-F968E554663A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
     <t>Bot_Wait_Time</t>
   </si>
   <si>
-    <t>Amount of time in seconds bot has to wait for user input before proceeding.</t>
+    <t>Amount of time in millisesondsbot has to wait for user input before proceeding.</t>
   </si>
 </sst>
 </file>
@@ -395,7 +395,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -421,7 +421,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>20000</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>

</xml_diff>